<commit_message>
Update documentation and README
</commit_message>
<xml_diff>
--- a/docs/CCTA BOM.xlsx
+++ b/docs/CCTA BOM.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yousu\OneDrive\Documents\McMaster University\Capstone\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mcmasteru365.sharepoint.com/sites/CapstoneGroup2/Shared Documents/General/BSC Compiled Files/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEF854A7-1E7F-4566-9EAB-2451E2E7FE43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{EEF854A7-1E7F-4566-9EAB-2451E2E7FE43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4D6BBF92-B609-48A1-BD65-F50202925EDE}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{8F13EF61-05BF-41EB-811E-FF093C2321EA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{8F13EF61-05BF-41EB-811E-FF093C2321EA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -305,9 +305,6 @@
     <t>Electrical</t>
   </si>
   <si>
-    <t>3/8" Quick Connect Water Flow Sensor Food-Grade</t>
-  </si>
-  <si>
     <t>Food Grade Plastic</t>
   </si>
   <si>
@@ -321,6 +318,9 @@
   </si>
   <si>
     <t xml:space="preserve">Mechanical </t>
+  </si>
+  <si>
+    <t>3/8" GREDIA Quick Connect Water Flow Sensor Food-Grade</t>
   </si>
 </sst>
 </file>
@@ -470,7 +470,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
@@ -499,22 +499,12 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -676,8 +666,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{4146374A-01F8-49EC-9554-31710E7E77E3}" name="Table2" displayName="Table2" ref="B1:L40" totalsRowShown="0" headerRowDxfId="13" dataDxfId="11" headerRowBorderDxfId="12" tableBorderDxfId="10">
-  <autoFilter ref="B1:L40" xr:uid="{4146374A-01F8-49EC-9554-31710E7E77E3}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{4146374A-01F8-49EC-9554-31710E7E77E3}" name="Table2" displayName="Table2" ref="B1:L39" totalsRowShown="0" headerRowDxfId="13" dataDxfId="11" headerRowBorderDxfId="12" tableBorderDxfId="10">
+  <autoFilter ref="B1:L39" xr:uid="{4146374A-01F8-49EC-9554-31710E7E77E3}"/>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{25039F7F-D8B0-41F4-828D-7E1C97A8BD5E}" name="Part Number" dataDxfId="9"/>
     <tableColumn id="2" xr3:uid="{39B32786-B2A2-420A-8358-BBCE23BE5E83}" name="Description" dataDxfId="8"/>
@@ -1012,29 +1002,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7C51E45-523D-4172-BD1E-FA2FC7DC84C2}">
-  <dimension ref="B1:L40"/>
+  <dimension ref="B1:L39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.53125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.06640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="49.53125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.3984375" customWidth="1"/>
-    <col min="5" max="5" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.06640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.19921875" customWidth="1"/>
-    <col min="8" max="8" width="14.3984375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.06640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.06640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.46484375" style="16" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="49.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" customWidth="1"/>
+    <col min="5" max="5" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.140625" customWidth="1"/>
+    <col min="8" max="8" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.85546875" style="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="2:12" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B1" s="7" t="s">
         <v>0</v>
       </c>
@@ -1065,11 +1055,11 @@
       <c r="K1" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="L1" s="12" t="s">
+      <c r="L1" s="8" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="2" spans="2:12" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="2" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="1">
         <v>1</v>
       </c>
@@ -1101,31 +1091,31 @@
       <c r="K2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="L2" s="13"/>
-    </row>
-    <row r="3" spans="2:12" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B3" s="10">
+      <c r="L2" s="10"/>
+    </row>
+    <row r="3" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="1">
         <v>2</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="2" t="s">
         <v>84</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="E3" s="11">
+      <c r="E3" s="2">
         <v>1</v>
       </c>
-      <c r="F3" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="G3" s="11" t="s">
+      <c r="F3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H3" s="11" t="s">
+      <c r="H3" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="I3" s="11">
+      <c r="I3" s="2">
         <v>39.99</v>
       </c>
       <c r="J3" s="2">
@@ -1135,9 +1125,9 @@
       <c r="K3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="L3" s="13"/>
-    </row>
-    <row r="4" spans="2:12" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="L3" s="10"/>
+    </row>
+    <row r="4" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="4">
         <v>3</v>
       </c>
@@ -1169,9 +1159,9 @@
       <c r="K4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="L4" s="13"/>
-    </row>
-    <row r="5" spans="2:12" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="L4" s="10"/>
+    </row>
+    <row r="5" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="1">
         <v>4</v>
       </c>
@@ -1201,12 +1191,12 @@
         <v>0</v>
       </c>
       <c r="K5" s="6"/>
-      <c r="L5" s="14" t="s">
+      <c r="L5" s="11" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="6" spans="2:12" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B6" s="10">
+    <row r="6" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="1">
         <v>5</v>
       </c>
       <c r="C6" s="5" t="s">
@@ -1235,11 +1225,11 @@
         <v>0</v>
       </c>
       <c r="K6" s="6"/>
-      <c r="L6" s="14" t="s">
+      <c r="L6" s="11" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="7" spans="2:12" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="7" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="4">
         <v>6</v>
       </c>
@@ -1269,46 +1259,46 @@
         <v>0</v>
       </c>
       <c r="K7" s="6"/>
-      <c r="L7" s="14" t="s">
+      <c r="L7" s="11" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="8" spans="2:12" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="8" spans="2:12" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="1">
         <v>7</v>
       </c>
-      <c r="C8" s="11" t="s">
-        <v>89</v>
+      <c r="C8" s="2" t="s">
+        <v>94</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="E8" s="11">
+      <c r="E8" s="2">
         <v>2</v>
       </c>
-      <c r="F8" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="G8" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="H8" s="11" t="s">
+      <c r="F8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="H8" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="I8" s="11">
+      <c r="I8" s="2">
         <v>14.99</v>
       </c>
       <c r="J8" s="2">
         <f>Table2[[#This Row],[Cost per Unit (CAD)]]*Table2[[#This Row],[Quantity]]</f>
         <v>29.98</v>
       </c>
-      <c r="K8" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="L8" s="14"/>
-    </row>
-    <row r="9" spans="2:12" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B9" s="10">
+      <c r="K8" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="L8" s="11"/>
+    </row>
+    <row r="9" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="1">
         <v>8</v>
       </c>
       <c r="C9" s="2" t="s">
@@ -1339,9 +1329,9 @@
       <c r="K9" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="L9" s="13"/>
-    </row>
-    <row r="10" spans="2:12" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="L9" s="10"/>
+    </row>
+    <row r="10" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="4">
         <v>9</v>
       </c>
@@ -1373,9 +1363,9 @@
       <c r="K10" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="L10" s="13"/>
-    </row>
-    <row r="11" spans="2:12" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="L10" s="10"/>
+    </row>
+    <row r="11" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="1">
         <v>10</v>
       </c>
@@ -1407,10 +1397,10 @@
       <c r="K11" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="L11" s="13"/>
-    </row>
-    <row r="12" spans="2:12" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B12" s="10">
+      <c r="L11" s="10"/>
+    </row>
+    <row r="12" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="1">
         <v>11</v>
       </c>
       <c r="C12" s="5" t="s">
@@ -1441,9 +1431,9 @@
       <c r="K12" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="L12" s="13"/>
-    </row>
-    <row r="13" spans="2:12" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="L12" s="10"/>
+    </row>
+    <row r="13" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="4">
         <v>12</v>
       </c>
@@ -1475,9 +1465,9 @@
       <c r="K13" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="L13" s="13"/>
-    </row>
-    <row r="14" spans="2:12" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="L13" s="10"/>
+    </row>
+    <row r="14" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="1">
         <v>13</v>
       </c>
@@ -1509,10 +1499,10 @@
       <c r="K14" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="L14" s="13"/>
-    </row>
-    <row r="15" spans="2:12" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B15" s="10">
+      <c r="L14" s="10"/>
+    </row>
+    <row r="15" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="1">
         <v>14</v>
       </c>
       <c r="C15" s="2" t="s">
@@ -1543,31 +1533,31 @@
       <c r="K15" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="L15" s="13"/>
-    </row>
-    <row r="16" spans="2:12" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="L15" s="10"/>
+    </row>
+    <row r="16" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="4">
         <v>15</v>
       </c>
-      <c r="C16" s="11" t="s">
+      <c r="C16" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="D16" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="D16" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="E16" s="11">
+      <c r="E16" s="2">
         <v>2</v>
       </c>
-      <c r="F16" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="G16" s="11" t="s">
+      <c r="F16" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G16" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H16" s="11" t="s">
+      <c r="H16" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="I16" s="11">
+      <c r="I16" s="2">
         <v>3.16</v>
       </c>
       <c r="J16" s="2">
@@ -1577,14 +1567,14 @@
       <c r="K16" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="L16" s="13"/>
-    </row>
-    <row r="17" spans="2:12" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="L16" s="10"/>
+    </row>
+    <row r="17" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="1">
         <v>16</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>77</v>
@@ -1611,10 +1601,10 @@
       <c r="K17" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="L17" s="13"/>
-    </row>
-    <row r="18" spans="2:12" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B18" s="10">
+      <c r="L17" s="10"/>
+    </row>
+    <row r="18" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="1">
         <v>17</v>
       </c>
       <c r="C18" s="5" t="s">
@@ -1645,9 +1635,9 @@
       <c r="K18" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="L18" s="13"/>
-    </row>
-    <row r="19" spans="2:12" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="L18" s="10"/>
+    </row>
+    <row r="19" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="4">
         <v>18</v>
       </c>
@@ -1679,9 +1669,9 @@
       <c r="K19" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="L19" s="13"/>
-    </row>
-    <row r="20" spans="2:12" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="L19" s="10"/>
+    </row>
+    <row r="20" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" s="1">
         <v>19</v>
       </c>
@@ -1713,10 +1703,10 @@
       <c r="K20" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="L20" s="13"/>
-    </row>
-    <row r="21" spans="2:12" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B21" s="10">
+      <c r="L20" s="10"/>
+    </row>
+    <row r="21" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="1">
         <v>20</v>
       </c>
       <c r="C21" s="2" t="s">
@@ -1747,9 +1737,9 @@
       <c r="K21" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="L21" s="13"/>
-    </row>
-    <row r="22" spans="2:12" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="L21" s="10"/>
+    </row>
+    <row r="22" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B22" s="4">
         <v>21</v>
       </c>
@@ -1781,9 +1771,9 @@
       <c r="K22" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="L22" s="13"/>
-    </row>
-    <row r="23" spans="2:12" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="L22" s="10"/>
+    </row>
+    <row r="23" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="1">
         <v>22</v>
       </c>
@@ -1815,10 +1805,10 @@
       <c r="K23" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="L23" s="13"/>
-    </row>
-    <row r="24" spans="2:12" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B24" s="10">
+      <c r="L23" s="10"/>
+    </row>
+    <row r="24" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="1">
         <v>23</v>
       </c>
       <c r="C24" s="5" t="s">
@@ -1849,9 +1839,9 @@
       <c r="K24" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="L24" s="13"/>
-    </row>
-    <row r="25" spans="2:12" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="L24" s="10"/>
+    </row>
+    <row r="25" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B25" s="4">
         <v>24</v>
       </c>
@@ -1883,9 +1873,9 @@
       <c r="K25" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="L25" s="13"/>
-    </row>
-    <row r="26" spans="2:12" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="L25" s="10"/>
+    </row>
+    <row r="26" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B26" s="1">
         <v>25</v>
       </c>
@@ -1917,10 +1907,10 @@
       <c r="K26" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="L26" s="13"/>
-    </row>
-    <row r="27" spans="2:12" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B27" s="10">
+      <c r="L26" s="10"/>
+    </row>
+    <row r="27" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="1">
         <v>26</v>
       </c>
       <c r="C27" s="2" t="s">
@@ -1949,11 +1939,11 @@
         <v>0</v>
       </c>
       <c r="K27" s="6"/>
-      <c r="L27" s="14" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="28" spans="2:12" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="L27" s="11" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="28" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B28" s="4">
         <v>27</v>
       </c>
@@ -1985,9 +1975,9 @@
       <c r="K28" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="L28" s="13"/>
-    </row>
-    <row r="29" spans="2:12" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="L28" s="10"/>
+    </row>
+    <row r="29" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B29" s="1">
         <v>28</v>
       </c>
@@ -2019,10 +2009,10 @@
       <c r="K29" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="L29" s="13"/>
-    </row>
-    <row r="30" spans="2:12" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B30" s="10">
+      <c r="L29" s="10"/>
+    </row>
+    <row r="30" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="1">
         <v>29</v>
       </c>
       <c r="C30" s="5" t="s">
@@ -2053,9 +2043,9 @@
       <c r="K30" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="L30" s="13"/>
-    </row>
-    <row r="31" spans="2:12" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="L30" s="10"/>
+    </row>
+    <row r="31" spans="2:12" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B31" s="4">
         <v>30</v>
       </c>
@@ -2087,9 +2077,9 @@
       <c r="K31" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="L31" s="13"/>
-    </row>
-    <row r="32" spans="2:12" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="L31" s="10"/>
+    </row>
+    <row r="32" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B32" s="1">
         <v>31</v>
       </c>
@@ -2121,10 +2111,10 @@
       <c r="K32" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="L32" s="13"/>
-    </row>
-    <row r="33" spans="2:12" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B33" s="10">
+      <c r="L32" s="10"/>
+    </row>
+    <row r="33" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B33" s="1">
         <v>32</v>
       </c>
       <c r="C33" s="2" t="s">
@@ -2155,9 +2145,9 @@
       <c r="K33" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="L33" s="13"/>
-    </row>
-    <row r="34" spans="2:12" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="L33" s="10"/>
+    </row>
+    <row r="34" spans="2:12" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B34" s="4">
         <v>33</v>
       </c>
@@ -2189,9 +2179,9 @@
       <c r="K34" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="L34" s="13"/>
-    </row>
-    <row r="35" spans="2:12" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="L34" s="10"/>
+    </row>
+    <row r="35" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B35" s="1">
         <v>34</v>
       </c>
@@ -2223,10 +2213,10 @@
       <c r="K35" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="L35" s="13"/>
-    </row>
-    <row r="36" spans="2:12" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B36" s="10">
+      <c r="L35" s="10"/>
+    </row>
+    <row r="36" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B36" s="1">
         <v>35</v>
       </c>
       <c r="C36" s="5" t="s">
@@ -2257,9 +2247,9 @@
       <c r="K36" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="L36" s="13"/>
-    </row>
-    <row r="37" spans="2:12" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="L36" s="10"/>
+    </row>
+    <row r="37" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B37" s="4">
         <v>36</v>
       </c>
@@ -2291,9 +2281,9 @@
       <c r="K37" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="L37" s="13"/>
-    </row>
-    <row r="38" spans="2:12" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="L37" s="10"/>
+    </row>
+    <row r="38" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B38" s="1">
         <v>37</v>
       </c>
@@ -2326,10 +2316,10 @@
       <c r="K38" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="L38" s="13"/>
-    </row>
-    <row r="39" spans="2:12" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B39" s="10">
+      <c r="L38" s="10"/>
+    </row>
+    <row r="39" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B39" s="1">
         <v>38</v>
       </c>
       <c r="C39" s="5" t="s">
@@ -2360,13 +2350,7 @@
       <c r="K39" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="L39" s="13"/>
-    </row>
-    <row r="40" spans="2:12" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B40" s="4">
-        <v>39</v>
-      </c>
-      <c r="L40" s="15"/>
+      <c r="L39" s="10"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -2621,15 +2605,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="19e0f530-f394-4669-814a-712a3dfd85f8" xsi:nil="true"/>
@@ -2640,14 +2615,49 @@
 </p:properties>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{421869AB-8054-4B49-B714-DDB9744B1588}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{421869AB-8054-4B49-B714-DDB9744B1588}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="fc364331-337d-4673-b2f9-5d6f37334e37"/>
+    <ds:schemaRef ds:uri="19e0f530-f394-4669-814a-712a3dfd85f8"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7411E58B-2516-478D-8B30-5E4C1B32AA48}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DFF86A59-67CA-4FFD-9E7D-DFCD883F89BE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="19e0f530-f394-4669-814a-712a3dfd85f8"/>
+    <ds:schemaRef ds:uri="fc364331-337d-4673-b2f9-5d6f37334e37"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DFF86A59-67CA-4FFD-9E7D-DFCD883F89BE}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7411E58B-2516-478D-8B30-5E4C1B32AA48}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>